<commit_message>
implementada insercion en el excel
</commit_message>
<xml_diff>
--- a/src/test/resources/test.xlsx
+++ b/src/test/resources/test.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t xml:space="preserve">Imagen</t>
   </si>
@@ -34,7 +34,7 @@
     <t xml:space="preserve">Titulo Ingles</t>
   </si>
   <si>
-    <t xml:space="preserve">Descripcioon</t>
+    <t xml:space="preserve">Descripcion</t>
   </si>
   <si>
     <t xml:space="preserve">Descipcion ingles</t>
@@ -58,10 +58,37 @@
     <t xml:space="preserve">Observaciones</t>
   </si>
   <si>
-    <t>1591706779997</t>
-  </si>
-  <si>
-    <t>1591706810294</t>
+    <t>el path</t>
+  </si>
+  <si>
+    <t>el title spanish</t>
+  </si>
+  <si>
+    <t>el title english</t>
+  </si>
+  <si>
+    <t>la desc spanish</t>
+  </si>
+  <si>
+    <t>la desc english</t>
+  </si>
+  <si>
+    <t>los tags spanish</t>
+  </si>
+  <si>
+    <t>los tags english</t>
+  </si>
+  <si>
+    <t>el status</t>
+  </si>
+  <si>
+    <t>los sites</t>
+  </si>
+  <si>
+    <t>la fecha de envio</t>
+  </si>
+  <si>
+    <t>los commentarios</t>
   </si>
 </sst>
 </file>
@@ -76,6 +103,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -152,20 +180,64 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="twoCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1285875</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>15874</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1" name="Picture 1" descr="Picture"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="true"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="1285875" cy="1285875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L1" activeCellId="0" sqref="L1"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1025" customWidth="false" hidden="false" style="0" width="11.52" collapsed="true" outlineLevel="0"/>
+    <col min="1" max="1" customWidth="true" hidden="false" style="0" width="20.0" collapsed="true" outlineLevel="0"/>
+    <col min="2" max="1025" customWidth="false" hidden="false" style="0" width="11.52" collapsed="true" outlineLevel="0"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -206,14 +278,40 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="s">
+    <row r="2" ht="100.0" customHeight="true">
+      <c r="A2"/>
+      <c r="B2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
+      <c r="C2" t="s">
         <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -224,5 +322,6 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
refactorizados los tests poniendoles en paquetes unitarios o de integracion
</commit_message>
<xml_diff>
--- a/src/test/resources/test.xlsx
+++ b/src/test/resources/test.xlsx
@@ -58,37 +58,37 @@
     <t xml:space="preserve">Observaciones</t>
   </si>
   <si>
-    <t>el path</t>
-  </si>
-  <si>
-    <t>el title spanish</t>
-  </si>
-  <si>
-    <t>el title english</t>
-  </si>
-  <si>
-    <t>la desc spanish</t>
-  </si>
-  <si>
-    <t>la desc english</t>
-  </si>
-  <si>
-    <t>los tags spanish</t>
-  </si>
-  <si>
-    <t>los tags english</t>
-  </si>
-  <si>
-    <t>el status</t>
-  </si>
-  <si>
-    <t>los sites</t>
-  </si>
-  <si>
-    <t>la fecha de envio</t>
-  </si>
-  <si>
-    <t>los commentarios</t>
+    <t xml:space="preserve">el path</t>
+  </si>
+  <si>
+    <t xml:space="preserve">el title spanish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">el title english</t>
+  </si>
+  <si>
+    <t xml:space="preserve">la desc spanish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">la desc english</t>
+  </si>
+  <si>
+    <t xml:space="preserve">los tags spanish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">los tags english</t>
+  </si>
+  <si>
+    <t xml:space="preserve">el status</t>
+  </si>
+  <si>
+    <t xml:space="preserve">los sites</t>
+  </si>
+  <si>
+    <t xml:space="preserve">la fecha de envio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">los commentarios</t>
   </si>
 </sst>
 </file>
@@ -182,40 +182,39 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <xdr:twoCellAnchor editAs="twoCell">
+  <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1285875</xdr:colOff>
+      <xdr:colOff>1285560</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>15874</xdr:rowOff>
+      <xdr:rowOff>15480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1" name="Picture 1" descr="Picture"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="true"/>
-        </xdr:cNvPicPr>
+        <xdr:cNvPr id="0" name="Picture 1" descr=""/>
+        <xdr:cNvPicPr/>
       </xdr:nvPicPr>
       <xdr:blipFill>
         <a:blip r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
+        <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="1285875" cy="1285875"/>
+          <a:off x="0" y="162720"/>
+          <a:ext cx="1285560" cy="1285200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -231,13 +230,13 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" customWidth="true" hidden="false" style="0" width="20.0" collapsed="true" outlineLevel="0"/>
-    <col min="2" max="1025" customWidth="false" hidden="false" style="0" width="11.52" collapsed="true" outlineLevel="0"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.99"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -278,39 +277,38 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" ht="100.0" customHeight="true">
-      <c r="A2"/>
-      <c r="B2" t="s">
+    <row r="2" customFormat="false" ht="100" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B2" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" s="0" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>